<commit_message>
weak boundary table finalize
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis_miRNA/GO_results_TAD/TAD_boundries_go_analyzes_mouse_specific_db.xlsx
+++ b/gene_ontology_analysis_miRNA/GO_results_TAD/TAD_boundries_go_analyzes_mouse_specific_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/gene_ontology_analysis_miRNA/GO_results_TAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4896115-680C-994E-A22F-80F6564C9F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2281013-4076-7A40-BC3A-E992D9BB5BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="1800" windowWidth="46280" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="520" windowWidth="46280" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strong_Boundaries_GO_Biologi" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="1623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="1631">
   <si>
     <t>Rank</t>
   </si>
@@ -4892,6 +4892,30 @@
   </si>
   <si>
     <t>NLGN1, CDH12, JCAD</t>
+  </si>
+  <si>
+    <t>Transcription initiation from RNA polymerase II promoter, DNA-templated transcription</t>
+  </si>
+  <si>
+    <t>DNA binding, transcription factor activity</t>
+  </si>
+  <si>
+    <t>T cell differentiation, negative regulation of B cell apoptotic process</t>
+  </si>
+  <si>
+    <t>Cytokine binding, immune receptor activity</t>
+  </si>
+  <si>
+    <t>Transmembrane transporter activity, sugar transporter activity</t>
+  </si>
+  <si>
+    <t>SLC2A8, GRAMD2A</t>
+  </si>
+  <si>
+    <t>Kinase activity, phosphatase activity</t>
+  </si>
+  <si>
+    <t>DAP, NLRC3, PPP2CA, MAP3K2</t>
   </si>
 </sst>
 </file>
@@ -5040,7 +5064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5061,13 +5085,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5106,6 +5123,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5874,7 +5897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -5902,14 +5925,14 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="18" t="s">
+      <c r="L16" s="8"/>
+      <c r="M16" s="15" t="s">
         <v>1490</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -5937,8 +5960,8 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="18" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="15" t="s">
         <v>1491</v>
       </c>
       <c r="N17" s="5"/>
@@ -5972,10 +5995,10 @@
       <c r="I18" s="2">
         <v>0</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="L18" s="9" t="s">
         <v>1489</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="15" t="s">
         <v>1492</v>
       </c>
       <c r="N18" s="5"/>
@@ -6009,14 +6032,14 @@
       <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="18" t="s">
+      <c r="L19" s="9"/>
+      <c r="M19" s="15" t="s">
         <v>1493</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -6044,8 +6067,8 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="18" t="s">
+      <c r="L20" s="9"/>
+      <c r="M20" s="15" t="s">
         <v>1494</v>
       </c>
       <c r="N20" s="5"/>
@@ -6079,14 +6102,14 @@
       <c r="I21" s="2">
         <v>0</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="18" t="s">
+      <c r="L21" s="10"/>
+      <c r="M21" s="15" t="s">
         <v>1495</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -6114,14 +6137,14 @@
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="18" t="s">
+      <c r="L22" s="8"/>
+      <c r="M22" s="15" t="s">
         <v>1496</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:18" ht="192" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -6149,21 +6172,21 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="18" t="s">
+      <c r="L23" s="9"/>
+      <c r="M23" s="15" t="s">
         <v>1497</v>
       </c>
       <c r="N23" s="5"/>
-      <c r="O23" s="24" t="s">
+      <c r="O23" s="21" t="s">
         <v>1528</v>
       </c>
-      <c r="P23" s="25" t="s">
+      <c r="P23" s="22" t="s">
         <v>1529</v>
       </c>
-      <c r="Q23" s="25" t="s">
+      <c r="Q23" s="22" t="s">
         <v>1530</v>
       </c>
-      <c r="R23" s="26" t="s">
+      <c r="R23" s="23" t="s">
         <v>1531</v>
       </c>
     </row>
@@ -6195,10 +6218,10 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="9" t="s">
         <v>1502</v>
       </c>
-      <c r="M24" s="18" t="s">
+      <c r="M24" s="15" t="s">
         <v>1498</v>
       </c>
       <c r="N24" s="5"/>
@@ -6232,14 +6255,14 @@
       <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="18" t="s">
+      <c r="L25" s="9"/>
+      <c r="M25" s="15" t="s">
         <v>1499</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -6267,8 +6290,8 @@
       <c r="I26" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="18" t="s">
+      <c r="L26" s="9"/>
+      <c r="M26" s="15" t="s">
         <v>1500</v>
       </c>
       <c r="N26" s="5"/>
@@ -6302,8 +6325,8 @@
       <c r="I27" s="2">
         <v>0</v>
       </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="18" t="s">
+      <c r="L27" s="10"/>
+      <c r="M27" s="15" t="s">
         <v>1501</v>
       </c>
       <c r="N27" s="5"/>
@@ -6337,14 +6360,14 @@
       <c r="I28" s="2">
         <v>0</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="18" t="s">
+      <c r="L28" s="8"/>
+      <c r="M28" s="15" t="s">
         <v>1503</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -6372,8 +6395,8 @@
       <c r="I29" s="2">
         <v>0</v>
       </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="18" t="s">
+      <c r="L29" s="9"/>
+      <c r="M29" s="15" t="s">
         <v>1504</v>
       </c>
       <c r="N29" s="5"/>
@@ -6407,10 +6430,10 @@
       <c r="I30" s="2">
         <v>0</v>
       </c>
-      <c r="L30" s="12" t="s">
+      <c r="L30" s="9" t="s">
         <v>1509</v>
       </c>
-      <c r="M30" s="18" t="s">
+      <c r="M30" s="15" t="s">
         <v>1505</v>
       </c>
       <c r="N30" s="5"/>
@@ -6444,14 +6467,14 @@
       <c r="I31" s="2">
         <v>0</v>
       </c>
-      <c r="L31" s="12"/>
-      <c r="M31" s="18" t="s">
+      <c r="L31" s="9"/>
+      <c r="M31" s="15" t="s">
         <v>1506</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
     </row>
-    <row r="32" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -6479,8 +6502,8 @@
       <c r="I32" s="2">
         <v>0</v>
       </c>
-      <c r="L32" s="12"/>
-      <c r="M32" s="18" t="s">
+      <c r="L32" s="9"/>
+      <c r="M32" s="15" t="s">
         <v>1507</v>
       </c>
       <c r="N32" s="5"/>
@@ -6514,14 +6537,14 @@
       <c r="I33" s="2">
         <v>0</v>
       </c>
-      <c r="L33" s="13"/>
-      <c r="M33" s="18" t="s">
+      <c r="L33" s="10"/>
+      <c r="M33" s="15" t="s">
         <v>1508</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -6549,14 +6572,14 @@
       <c r="I34" s="2">
         <v>0</v>
       </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="18" t="s">
+      <c r="L34" s="8"/>
+      <c r="M34" s="15" t="s">
         <v>1510</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -6584,8 +6607,8 @@
       <c r="I35" s="2">
         <v>0</v>
       </c>
-      <c r="L35" s="12"/>
-      <c r="M35" s="18" t="s">
+      <c r="L35" s="9"/>
+      <c r="M35" s="15" t="s">
         <v>1511</v>
       </c>
       <c r="N35" s="5"/>
@@ -6619,16 +6642,16 @@
       <c r="I36" s="2">
         <v>0</v>
       </c>
-      <c r="L36" s="12" t="s">
+      <c r="L36" s="9" t="s">
         <v>1515</v>
       </c>
-      <c r="M36" s="18" t="s">
+      <c r="M36" s="15" t="s">
         <v>1512</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
     </row>
-    <row r="37" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -6656,8 +6679,8 @@
       <c r="I37" s="2">
         <v>0</v>
       </c>
-      <c r="L37" s="12"/>
-      <c r="M37" s="18" t="s">
+      <c r="L37" s="9"/>
+      <c r="M37" s="15" t="s">
         <v>1513</v>
       </c>
       <c r="N37" s="5"/>
@@ -6691,8 +6714,8 @@
       <c r="I38" s="2">
         <v>0</v>
       </c>
-      <c r="L38" s="13"/>
-      <c r="M38" s="18" t="s">
+      <c r="L38" s="10"/>
+      <c r="M38" s="15" t="s">
         <v>1514</v>
       </c>
       <c r="N38" s="5"/>
@@ -6726,8 +6749,8 @@
       <c r="I39" s="2">
         <v>0</v>
       </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="18" t="s">
+      <c r="L39" s="8"/>
+      <c r="M39" s="15" t="s">
         <v>1516</v>
       </c>
       <c r="N39" s="5"/>
@@ -6761,8 +6784,8 @@
       <c r="I40" s="2">
         <v>0</v>
       </c>
-      <c r="L40" s="12"/>
-      <c r="M40" s="18" t="s">
+      <c r="L40" s="9"/>
+      <c r="M40" s="15" t="s">
         <v>1517</v>
       </c>
       <c r="N40" s="5"/>
@@ -6796,16 +6819,16 @@
       <c r="I41" s="2">
         <v>0</v>
       </c>
-      <c r="L41" s="12" t="s">
+      <c r="L41" s="9" t="s">
         <v>1521</v>
       </c>
-      <c r="M41" s="18" t="s">
+      <c r="M41" s="15" t="s">
         <v>1518</v>
       </c>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
     </row>
-    <row r="42" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -6833,8 +6856,8 @@
       <c r="I42" s="2">
         <v>0</v>
       </c>
-      <c r="L42" s="14"/>
-      <c r="M42" s="18" t="s">
+      <c r="L42" s="11"/>
+      <c r="M42" s="15" t="s">
         <v>1519</v>
       </c>
     </row>
@@ -6866,12 +6889,12 @@
       <c r="I43" s="2">
         <v>0</v>
       </c>
-      <c r="L43" s="14"/>
-      <c r="M43" s="18" t="s">
+      <c r="L43" s="11"/>
+      <c r="M43" s="15" t="s">
         <v>1520</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -6899,8 +6922,8 @@
       <c r="I44" s="2">
         <v>0</v>
       </c>
-      <c r="L44" s="15"/>
-      <c r="M44" s="19" t="s">
+      <c r="L44" s="12"/>
+      <c r="M44" s="16" t="s">
         <v>1522</v>
       </c>
     </row>
@@ -6932,8 +6955,8 @@
       <c r="I45" s="2">
         <v>0</v>
       </c>
-      <c r="L45" s="14"/>
-      <c r="M45" s="19" t="s">
+      <c r="L45" s="11"/>
+      <c r="M45" s="16" t="s">
         <v>1523</v>
       </c>
     </row>
@@ -6965,10 +6988,10 @@
       <c r="I46" s="2">
         <v>0</v>
       </c>
-      <c r="L46" s="16" t="s">
+      <c r="L46" s="13" t="s">
         <v>1527</v>
       </c>
-      <c r="M46" s="19" t="s">
+      <c r="M46" s="16" t="s">
         <v>1524</v>
       </c>
     </row>
@@ -7000,8 +7023,8 @@
       <c r="I47" s="2">
         <v>0</v>
       </c>
-      <c r="L47" s="14"/>
-      <c r="M47" s="19" t="s">
+      <c r="L47" s="11"/>
+      <c r="M47" s="16" t="s">
         <v>1525</v>
       </c>
     </row>
@@ -7033,8 +7056,8 @@
       <c r="I48" s="2">
         <v>0</v>
       </c>
-      <c r="L48" s="17"/>
-      <c r="M48" s="19" t="s">
+      <c r="L48" s="14"/>
+      <c r="M48" s="16" t="s">
         <v>1526</v>
       </c>
     </row>
@@ -26525,8 +26548,8 @@
       <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="22" t="s">
+      <c r="L25" s="8"/>
+      <c r="M25" s="19" t="s">
         <v>1532</v>
       </c>
       <c r="P25" s="6" t="s">
@@ -26570,22 +26593,22 @@
       <c r="I26" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="L26" s="9" t="s">
         <v>1535</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="19" t="s">
         <v>1533</v>
       </c>
-      <c r="P26" s="18" t="s">
+      <c r="P26" s="15" t="s">
         <v>1535</v>
       </c>
-      <c r="Q26" s="18" t="s">
+      <c r="Q26" s="15" t="s">
         <v>1566</v>
       </c>
-      <c r="R26" s="18" t="s">
+      <c r="R26" s="15" t="s">
         <v>1567</v>
       </c>
-      <c r="S26" s="18" t="s">
+      <c r="S26" s="15" t="s">
         <v>1585</v>
       </c>
       <c r="T26" s="5"/>
@@ -26618,20 +26641,20 @@
       <c r="I27" s="2">
         <v>0</v>
       </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="22" t="s">
+      <c r="L27" s="10"/>
+      <c r="M27" s="19" t="s">
         <v>1534</v>
       </c>
-      <c r="P27" s="18" t="s">
+      <c r="P27" s="15" t="s">
         <v>1489</v>
       </c>
-      <c r="Q27" s="18" t="s">
+      <c r="Q27" s="15" t="s">
         <v>1568</v>
       </c>
-      <c r="R27" s="18" t="s">
+      <c r="R27" s="15" t="s">
         <v>1569</v>
       </c>
-      <c r="S27" s="18" t="s">
+      <c r="S27" s="15" t="s">
         <v>1586</v>
       </c>
       <c r="T27" s="5"/>
@@ -26664,20 +26687,20 @@
       <c r="I28" s="2">
         <v>0</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="22" t="s">
+      <c r="L28" s="8"/>
+      <c r="M28" s="19" t="s">
         <v>1536</v>
       </c>
-      <c r="P28" s="18" t="s">
+      <c r="P28" s="15" t="s">
         <v>1587</v>
       </c>
-      <c r="Q28" s="18" t="s">
+      <c r="Q28" s="15" t="s">
         <v>1570</v>
       </c>
-      <c r="R28" s="18" t="s">
+      <c r="R28" s="15" t="s">
         <v>1571</v>
       </c>
-      <c r="S28" s="18" t="s">
+      <c r="S28" s="15" t="s">
         <v>1588</v>
       </c>
       <c r="T28" s="5"/>
@@ -26710,22 +26733,22 @@
       <c r="I29" s="2">
         <v>0</v>
       </c>
-      <c r="L29" s="12" t="s">
+      <c r="L29" s="9" t="s">
         <v>1540</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="19" t="s">
         <v>1537</v>
       </c>
-      <c r="P29" s="18" t="s">
+      <c r="P29" s="15" t="s">
         <v>1509</v>
       </c>
-      <c r="Q29" s="18" t="s">
+      <c r="Q29" s="15" t="s">
         <v>1572</v>
       </c>
-      <c r="R29" s="18" t="s">
+      <c r="R29" s="15" t="s">
         <v>1573</v>
       </c>
-      <c r="S29" s="18" t="s">
+      <c r="S29" s="15" t="s">
         <v>1589</v>
       </c>
       <c r="T29" s="5"/>
@@ -26758,20 +26781,20 @@
       <c r="I30" s="2">
         <v>0</v>
       </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="22" t="s">
+      <c r="L30" s="9"/>
+      <c r="M30" s="19" t="s">
         <v>1538</v>
       </c>
-      <c r="P30" s="18" t="s">
+      <c r="P30" s="15" t="s">
         <v>1527</v>
       </c>
-      <c r="Q30" s="18" t="s">
+      <c r="Q30" s="15" t="s">
         <v>1574</v>
       </c>
-      <c r="R30" s="18" t="s">
+      <c r="R30" s="15" t="s">
         <v>1575</v>
       </c>
-      <c r="S30" s="18" t="s">
+      <c r="S30" s="15" t="s">
         <v>1590</v>
       </c>
       <c r="T30" s="5"/>
@@ -26804,20 +26827,20 @@
       <c r="I31" s="2">
         <v>0</v>
       </c>
-      <c r="L31" s="13"/>
-      <c r="M31" s="22" t="s">
+      <c r="L31" s="10"/>
+      <c r="M31" s="19" t="s">
         <v>1539</v>
       </c>
-      <c r="P31" s="18" t="s">
+      <c r="P31" s="15" t="s">
         <v>1550</v>
       </c>
-      <c r="Q31" s="18" t="s">
+      <c r="Q31" s="15" t="s">
         <v>1576</v>
       </c>
-      <c r="R31" s="18" t="s">
+      <c r="R31" s="15" t="s">
         <v>1577</v>
       </c>
-      <c r="S31" s="18" t="s">
+      <c r="S31" s="15" t="s">
         <v>1591</v>
       </c>
       <c r="T31" s="5"/>
@@ -26850,20 +26873,20 @@
       <c r="I32" s="2">
         <v>0</v>
       </c>
-      <c r="L32" s="20"/>
-      <c r="M32" s="22" t="s">
+      <c r="L32" s="17"/>
+      <c r="M32" s="19" t="s">
         <v>1541</v>
       </c>
-      <c r="P32" s="18" t="s">
+      <c r="P32" s="15" t="s">
         <v>1592</v>
       </c>
-      <c r="Q32" s="18" t="s">
+      <c r="Q32" s="15" t="s">
         <v>1578</v>
       </c>
-      <c r="R32" s="18" t="s">
+      <c r="R32" s="15" t="s">
         <v>1579</v>
       </c>
-      <c r="S32" s="18" t="s">
+      <c r="S32" s="15" t="s">
         <v>1593</v>
       </c>
       <c r="T32" s="5"/>
@@ -26896,22 +26919,22 @@
       <c r="I33" s="2">
         <v>0</v>
       </c>
-      <c r="L33" s="16" t="s">
+      <c r="L33" s="13" t="s">
         <v>1545</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="M33" s="19" t="s">
         <v>1542</v>
       </c>
-      <c r="P33" s="18" t="s">
+      <c r="P33" s="15" t="s">
         <v>1594</v>
       </c>
-      <c r="Q33" s="18" t="s">
+      <c r="Q33" s="15" t="s">
         <v>1580</v>
       </c>
-      <c r="R33" s="18" t="s">
+      <c r="R33" s="15" t="s">
         <v>1581</v>
       </c>
-      <c r="S33" s="18" t="s">
+      <c r="S33" s="15" t="s">
         <v>1582</v>
       </c>
       <c r="T33" s="5"/>
@@ -26944,14 +26967,14 @@
       <c r="I34" s="2">
         <v>0</v>
       </c>
-      <c r="L34" s="16"/>
-      <c r="M34" s="22" t="s">
+      <c r="L34" s="13"/>
+      <c r="M34" s="19" t="s">
         <v>1543</v>
       </c>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
       <c r="T34" s="5"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -26982,14 +27005,14 @@
       <c r="I35" s="2">
         <v>0</v>
       </c>
-      <c r="L35" s="21"/>
-      <c r="M35" s="22" t="s">
+      <c r="L35" s="18"/>
+      <c r="M35" s="19" t="s">
         <v>1544</v>
       </c>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -27020,14 +27043,14 @@
       <c r="I36" s="2">
         <v>0</v>
       </c>
-      <c r="L36" s="20"/>
-      <c r="M36" s="22" t="s">
+      <c r="L36" s="17"/>
+      <c r="M36" s="19" t="s">
         <v>1546</v>
       </c>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
       <c r="T36" s="5"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -27058,14 +27081,14 @@
       <c r="I37" s="2">
         <v>0</v>
       </c>
-      <c r="L37" s="16"/>
-      <c r="M37" s="22" t="s">
+      <c r="L37" s="13"/>
+      <c r="M37" s="19" t="s">
         <v>1547</v>
       </c>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
       <c r="T37" s="5"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -27096,16 +27119,16 @@
       <c r="I38" s="2">
         <v>0</v>
       </c>
-      <c r="L38" s="16" t="s">
+      <c r="L38" s="13" t="s">
         <v>1550</v>
       </c>
-      <c r="M38" s="22" t="s">
+      <c r="M38" s="19" t="s">
         <v>1548</v>
       </c>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
       <c r="T38" s="5"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
@@ -27136,14 +27159,14 @@
       <c r="I39" s="2">
         <v>0</v>
       </c>
-      <c r="L39" s="21"/>
-      <c r="M39" s="22" t="s">
+      <c r="L39" s="18"/>
+      <c r="M39" s="19" t="s">
         <v>1549</v>
       </c>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
       <c r="T39" s="5"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -27174,14 +27197,14 @@
       <c r="I40" s="2">
         <v>0</v>
       </c>
-      <c r="L40" s="11"/>
-      <c r="M40" s="23" t="s">
+      <c r="L40" s="8"/>
+      <c r="M40" s="20" t="s">
         <v>1551</v>
       </c>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
       <c r="T40" s="5"/>
     </row>
     <row r="41" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -27212,16 +27235,16 @@
       <c r="I41" s="2">
         <v>0</v>
       </c>
-      <c r="L41" s="12" t="s">
+      <c r="L41" s="9" t="s">
         <v>1554</v>
       </c>
-      <c r="M41" s="23" t="s">
+      <c r="M41" s="20" t="s">
         <v>1552</v>
       </c>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
       <c r="T41" s="5"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -27252,14 +27275,10 @@
       <c r="I42" s="2">
         <v>0</v>
       </c>
-      <c r="L42" s="13"/>
-      <c r="M42" s="23" t="s">
+      <c r="L42" s="10"/>
+      <c r="M42" s="20" t="s">
         <v>1553</v>
       </c>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -27289,14 +27308,10 @@
       <c r="I43" s="2">
         <v>0</v>
       </c>
-      <c r="L43" s="20"/>
-      <c r="M43" s="23" t="s">
+      <c r="L43" s="17"/>
+      <c r="M43" s="20" t="s">
         <v>1555</v>
       </c>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
     </row>
     <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
@@ -27326,16 +27341,12 @@
       <c r="I44" s="2">
         <v>0</v>
       </c>
-      <c r="L44" s="12" t="s">
+      <c r="L44" s="9" t="s">
         <v>1558</v>
       </c>
-      <c r="M44" s="23" t="s">
+      <c r="M44" s="20" t="s">
         <v>1556</v>
       </c>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -27365,8 +27376,8 @@
       <c r="I45" s="2">
         <v>0</v>
       </c>
-      <c r="L45" s="21"/>
-      <c r="M45" s="23" t="s">
+      <c r="L45" s="18"/>
+      <c r="M45" s="20" t="s">
         <v>1557</v>
       </c>
     </row>
@@ -27398,8 +27409,8 @@
       <c r="I46" s="2">
         <v>0</v>
       </c>
-      <c r="L46" s="11"/>
-      <c r="M46" s="23" t="s">
+      <c r="L46" s="8"/>
+      <c r="M46" s="20" t="s">
         <v>1559</v>
       </c>
     </row>
@@ -27431,8 +27442,8 @@
       <c r="I47" s="2">
         <v>0</v>
       </c>
-      <c r="L47" s="12"/>
-      <c r="M47" s="23" t="s">
+      <c r="L47" s="9"/>
+      <c r="M47" s="20" t="s">
         <v>1560</v>
       </c>
     </row>
@@ -27464,10 +27475,10 @@
       <c r="I48" s="2">
         <v>0</v>
       </c>
-      <c r="L48" s="12" t="s">
+      <c r="L48" s="9" t="s">
         <v>1563</v>
       </c>
-      <c r="M48" s="23" t="s">
+      <c r="M48" s="20" t="s">
         <v>1561</v>
       </c>
     </row>
@@ -27499,8 +27510,8 @@
       <c r="I49" s="2">
         <v>0</v>
       </c>
-      <c r="L49" s="13"/>
-      <c r="M49" s="23" t="s">
+      <c r="L49" s="10"/>
+      <c r="M49" s="20" t="s">
         <v>1562</v>
       </c>
     </row>
@@ -30547,7 +30558,7 @@
     <col min="15" max="16" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -30576,7 +30587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -30605,7 +30616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -30634,7 +30645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -30663,7 +30674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -30692,7 +30703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -30721,7 +30732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -30750,7 +30761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -30779,7 +30790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -30811,7 +30822,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -30839,11 +30850,11 @@
       <c r="I10" s="2">
         <v>0</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="15" t="s">
         <v>1488</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -30872,7 +30883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -30901,7 +30912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -30930,7 +30941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -30959,7 +30970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -30988,7 +30999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -31016,9 +31027,6 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -31086,13 +31094,13 @@
       <c r="I18" s="2">
         <v>0</v>
       </c>
-      <c r="N18" s="18" t="s">
+      <c r="N18" s="15" t="s">
         <v>1595</v>
       </c>
-      <c r="O18" s="18" t="s">
+      <c r="O18" s="15" t="s">
         <v>1596</v>
       </c>
-      <c r="P18" s="18" t="s">
+      <c r="P18" s="15" t="s">
         <v>1597</v>
       </c>
     </row>
@@ -31124,9 +31132,9 @@
       <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
     </row>
     <row r="20" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -31159,13 +31167,13 @@
       <c r="L20" t="s">
         <v>1614</v>
       </c>
-      <c r="N20" s="18" t="s">
+      <c r="N20" s="15" t="s">
         <v>1598</v>
       </c>
-      <c r="O20" s="18" t="s">
+      <c r="O20" s="15" t="s">
         <v>1599</v>
       </c>
-      <c r="P20" s="18" t="s">
+      <c r="P20" s="15" t="s">
         <v>1600</v>
       </c>
     </row>
@@ -31197,13 +31205,13 @@
       <c r="I21" s="2">
         <v>0</v>
       </c>
-      <c r="N21" s="18" t="s">
+      <c r="N21" s="15" t="s">
         <v>1601</v>
       </c>
-      <c r="O21" s="18" t="s">
+      <c r="O21" s="15" t="s">
         <v>1602</v>
       </c>
-      <c r="P21" s="18" t="s">
+      <c r="P21" s="15" t="s">
         <v>1603</v>
       </c>
     </row>
@@ -31235,13 +31243,13 @@
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="N22" s="18" t="s">
+      <c r="N22" s="15" t="s">
         <v>1535</v>
       </c>
-      <c r="O22" s="18" t="s">
+      <c r="O22" s="15" t="s">
         <v>1604</v>
       </c>
-      <c r="P22" s="18" t="s">
+      <c r="P22" s="15" t="s">
         <v>1605</v>
       </c>
     </row>
@@ -31273,13 +31281,13 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="N23" s="18" t="s">
+      <c r="N23" s="15" t="s">
         <v>1489</v>
       </c>
-      <c r="O23" s="18" t="s">
+      <c r="O23" s="15" t="s">
         <v>1608</v>
       </c>
-      <c r="P23" s="18" t="s">
+      <c r="P23" s="15" t="s">
         <v>1609</v>
       </c>
     </row>
@@ -31311,13 +31319,13 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
-      <c r="N24" s="18" t="s">
+      <c r="N24" s="15" t="s">
         <v>1606</v>
       </c>
-      <c r="O24" s="18" t="s">
+      <c r="O24" s="15" t="s">
         <v>1610</v>
       </c>
-      <c r="P24" s="18" t="s">
+      <c r="P24" s="15" t="s">
         <v>1611</v>
       </c>
     </row>
@@ -31349,13 +31357,13 @@
       <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="N25" s="15" t="s">
         <v>1607</v>
       </c>
-      <c r="O25" s="18" t="s">
+      <c r="O25" s="15" t="s">
         <v>1612</v>
       </c>
-      <c r="P25" s="18" t="s">
+      <c r="P25" s="15" t="s">
         <v>1613</v>
       </c>
     </row>
@@ -44489,7 +44497,7 @@
   <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44502,9 +44510,9 @@
     <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.33203125" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.6640625" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -44912,20 +44920,20 @@
       <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="25" t="s">
         <v>1564</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="P14" s="25" t="s">
         <v>1583</v>
       </c>
-      <c r="Q14" s="8" t="s">
+      <c r="Q14" s="25" t="s">
         <v>1615</v>
       </c>
-      <c r="R14" s="8" t="s">
+      <c r="R14" s="25" t="s">
         <v>1584</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="96" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -44953,16 +44961,16 @@
       <c r="I15" s="2">
         <v>0</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="O15" s="15" t="s">
         <v>1616</v>
       </c>
-      <c r="P15" s="8" t="s">
+      <c r="P15" s="15" t="s">
         <v>1596</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="Q15" s="15" t="s">
         <v>1617</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="15" t="s">
         <v>1618</v>
       </c>
     </row>
@@ -44994,16 +45002,16 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="15" t="s">
         <v>1619</v>
       </c>
-      <c r="P16" s="8" t="s">
+      <c r="P16" s="15" t="s">
         <v>1599</v>
       </c>
-      <c r="Q16" s="8" t="s">
+      <c r="Q16" s="15" t="s">
         <v>1620</v>
       </c>
-      <c r="R16" s="8" t="s">
+      <c r="R16" s="15" t="s">
         <v>1600</v>
       </c>
     </row>
@@ -45035,20 +45043,20 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="O17" s="15" t="s">
         <v>1601</v>
       </c>
-      <c r="P17" s="8" t="s">
+      <c r="P17" s="15" t="s">
         <v>1602</v>
       </c>
-      <c r="Q17" s="8" t="s">
+      <c r="Q17" s="15" t="s">
         <v>1621</v>
       </c>
-      <c r="R17" s="8" t="s">
+      <c r="R17" s="15" t="s">
         <v>1622</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="128" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -45076,12 +45084,20 @@
       <c r="I18" s="2">
         <v>0</v>
       </c>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O18" s="15" t="s">
+        <v>1535</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>1623</v>
+      </c>
+      <c r="Q18" s="15" t="s">
+        <v>1624</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -45109,12 +45125,20 @@
       <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O19" s="15" t="s">
+        <v>1489</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>1625</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>1626</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -45142,12 +45166,20 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O20" s="15" t="s">
+        <v>1606</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>1610</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>1627</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -45175,10 +45207,18 @@
       <c r="I21" s="2">
         <v>0</v>
       </c>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+      <c r="O21" s="15" t="s">
+        <v>1607</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>1612</v>
+      </c>
+      <c r="Q21" s="15" t="s">
+        <v>1629</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>1630</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -45208,10 +45248,10 @@
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
@@ -45241,10 +45281,10 @@
       <c r="I23" s="2">
         <v>0</v>
       </c>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
@@ -45274,10 +45314,10 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">

</xml_diff>

<commit_message>
highest performed model with lr 0.0008/epoch 60
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis_miRNA/GO_results_TAD/TAD_boundries_go_analyzes_mouse_specific_db.xlsx
+++ b/gene_ontology_analysis_miRNA/GO_results_TAD/TAD_boundries_go_analyzes_mouse_specific_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/gene_ontology_analysis_miRNA/GO_results_TAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2281013-4076-7A40-BC3A-E992D9BB5BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B15A48-9E1B-FC48-A433-787296208DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="520" windowWidth="46280" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="500" windowWidth="39520" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strong_Boundaries_GO_Biologi" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="1631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="1633">
   <si>
     <t>Rank</t>
   </si>
@@ -4720,9 +4720,6 @@
     <t>Functional Category</t>
   </si>
   <si>
-    <t>Key Molecular Functions</t>
-  </si>
-  <si>
     <t>RNA processing, mRNA stabilization, miRNA regulation</t>
   </si>
   <si>
@@ -4870,9 +4867,6 @@
     <t>s</t>
   </si>
   <si>
-    <t>Key Functions</t>
-  </si>
-  <si>
     <t>RNA Processing</t>
   </si>
   <si>
@@ -4916,6 +4910,18 @@
   </si>
   <si>
     <t>DAP, NLRC3, PPP2CA, MAP3K2</t>
+  </si>
+  <si>
+    <t>Generalized Tabel for Strong Boundaries with Biological and Molecular Aspects</t>
+  </si>
+  <si>
+    <t>Generalized Table for Weak Boundaries with Biological and Molecular Aspects</t>
+  </si>
+  <si>
+    <t>Biological Process</t>
+  </si>
+  <si>
+    <t>Molecular Functions</t>
   </si>
 </sst>
 </file>
@@ -4937,7 +4943,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4959,6 +4965,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5064,7 +5076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5125,10 +5137,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5435,7 +5450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R694"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F9" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="F12" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
@@ -25804,8 +25819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T153"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView showGridLines="0" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26519,6 +26534,9 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
+      <c r="P24" t="s">
+        <v>1629</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -26552,17 +26570,17 @@
       <c r="M25" s="19" t="s">
         <v>1532</v>
       </c>
-      <c r="P25" s="6" t="s">
+      <c r="P25" s="24" t="s">
         <v>1564</v>
       </c>
-      <c r="Q25" s="6" t="s">
+      <c r="Q25" s="24" t="s">
+        <v>1631</v>
+      </c>
+      <c r="R25" s="24" t="s">
+        <v>1632</v>
+      </c>
+      <c r="S25" s="24" t="s">
         <v>1583</v>
-      </c>
-      <c r="R25" s="6" t="s">
-        <v>1565</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>1584</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="80" x14ac:dyDescent="0.2">
@@ -26599,17 +26617,17 @@
       <c r="M26" s="19" t="s">
         <v>1533</v>
       </c>
-      <c r="P26" s="15" t="s">
+      <c r="P26" s="25" t="s">
         <v>1535</v>
       </c>
-      <c r="Q26" s="15" t="s">
+      <c r="Q26" s="25" t="s">
+        <v>1565</v>
+      </c>
+      <c r="R26" s="25" t="s">
         <v>1566</v>
       </c>
-      <c r="R26" s="15" t="s">
-        <v>1567</v>
-      </c>
-      <c r="S26" s="15" t="s">
-        <v>1585</v>
+      <c r="S26" s="25" t="s">
+        <v>1584</v>
       </c>
       <c r="T26" s="5"/>
     </row>
@@ -26645,17 +26663,17 @@
       <c r="M27" s="19" t="s">
         <v>1534</v>
       </c>
-      <c r="P27" s="15" t="s">
+      <c r="P27" s="25" t="s">
         <v>1489</v>
       </c>
-      <c r="Q27" s="15" t="s">
+      <c r="Q27" s="25" t="s">
+        <v>1567</v>
+      </c>
+      <c r="R27" s="25" t="s">
         <v>1568</v>
       </c>
-      <c r="R27" s="15" t="s">
-        <v>1569</v>
-      </c>
-      <c r="S27" s="15" t="s">
-        <v>1586</v>
+      <c r="S27" s="25" t="s">
+        <v>1585</v>
       </c>
       <c r="T27" s="5"/>
     </row>
@@ -26691,17 +26709,17 @@
       <c r="M28" s="19" t="s">
         <v>1536</v>
       </c>
-      <c r="P28" s="15" t="s">
+      <c r="P28" s="25" t="s">
+        <v>1586</v>
+      </c>
+      <c r="Q28" s="25" t="s">
+        <v>1569</v>
+      </c>
+      <c r="R28" s="25" t="s">
+        <v>1570</v>
+      </c>
+      <c r="S28" s="25" t="s">
         <v>1587</v>
-      </c>
-      <c r="Q28" s="15" t="s">
-        <v>1570</v>
-      </c>
-      <c r="R28" s="15" t="s">
-        <v>1571</v>
-      </c>
-      <c r="S28" s="15" t="s">
-        <v>1588</v>
       </c>
       <c r="T28" s="5"/>
     </row>
@@ -26739,17 +26757,17 @@
       <c r="M29" s="19" t="s">
         <v>1537</v>
       </c>
-      <c r="P29" s="15" t="s">
+      <c r="P29" s="25" t="s">
         <v>1509</v>
       </c>
-      <c r="Q29" s="15" t="s">
+      <c r="Q29" s="25" t="s">
+        <v>1571</v>
+      </c>
+      <c r="R29" s="25" t="s">
         <v>1572</v>
       </c>
-      <c r="R29" s="15" t="s">
-        <v>1573</v>
-      </c>
-      <c r="S29" s="15" t="s">
-        <v>1589</v>
+      <c r="S29" s="25" t="s">
+        <v>1588</v>
       </c>
       <c r="T29" s="5"/>
     </row>
@@ -26785,17 +26803,17 @@
       <c r="M30" s="19" t="s">
         <v>1538</v>
       </c>
-      <c r="P30" s="15" t="s">
+      <c r="P30" s="25" t="s">
         <v>1527</v>
       </c>
-      <c r="Q30" s="15" t="s">
+      <c r="Q30" s="25" t="s">
+        <v>1573</v>
+      </c>
+      <c r="R30" s="25" t="s">
         <v>1574</v>
       </c>
-      <c r="R30" s="15" t="s">
-        <v>1575</v>
-      </c>
-      <c r="S30" s="15" t="s">
-        <v>1590</v>
+      <c r="S30" s="25" t="s">
+        <v>1589</v>
       </c>
       <c r="T30" s="5"/>
     </row>
@@ -26831,17 +26849,17 @@
       <c r="M31" s="19" t="s">
         <v>1539</v>
       </c>
-      <c r="P31" s="15" t="s">
+      <c r="P31" s="25" t="s">
         <v>1550</v>
       </c>
-      <c r="Q31" s="15" t="s">
+      <c r="Q31" s="25" t="s">
+        <v>1575</v>
+      </c>
+      <c r="R31" s="25" t="s">
         <v>1576</v>
       </c>
-      <c r="R31" s="15" t="s">
-        <v>1577</v>
-      </c>
-      <c r="S31" s="15" t="s">
-        <v>1591</v>
+      <c r="S31" s="25" t="s">
+        <v>1590</v>
       </c>
       <c r="T31" s="5"/>
     </row>
@@ -26877,17 +26895,17 @@
       <c r="M32" s="19" t="s">
         <v>1541</v>
       </c>
-      <c r="P32" s="15" t="s">
+      <c r="P32" s="25" t="s">
+        <v>1591</v>
+      </c>
+      <c r="Q32" s="25" t="s">
+        <v>1577</v>
+      </c>
+      <c r="R32" s="25" t="s">
+        <v>1578</v>
+      </c>
+      <c r="S32" s="25" t="s">
         <v>1592</v>
-      </c>
-      <c r="Q32" s="15" t="s">
-        <v>1578</v>
-      </c>
-      <c r="R32" s="15" t="s">
-        <v>1579</v>
-      </c>
-      <c r="S32" s="15" t="s">
-        <v>1593</v>
       </c>
       <c r="T32" s="5"/>
     </row>
@@ -26925,17 +26943,17 @@
       <c r="M33" s="19" t="s">
         <v>1542</v>
       </c>
-      <c r="P33" s="15" t="s">
-        <v>1594</v>
-      </c>
-      <c r="Q33" s="15" t="s">
+      <c r="P33" s="25" t="s">
+        <v>1593</v>
+      </c>
+      <c r="Q33" s="25" t="s">
+        <v>1579</v>
+      </c>
+      <c r="R33" s="25" t="s">
         <v>1580</v>
       </c>
-      <c r="R33" s="15" t="s">
+      <c r="S33" s="25" t="s">
         <v>1581</v>
-      </c>
-      <c r="S33" s="15" t="s">
-        <v>1582</v>
       </c>
       <c r="T33" s="5"/>
     </row>
@@ -30540,7 +30558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P477"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -31060,10 +31078,10 @@
         <v>1564</v>
       </c>
       <c r="O17" s="6" t="s">
+        <v>1582</v>
+      </c>
+      <c r="P17" s="6" t="s">
         <v>1583</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>1584</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="80" x14ac:dyDescent="0.2">
@@ -31095,13 +31113,13 @@
         <v>0</v>
       </c>
       <c r="N18" s="15" t="s">
+        <v>1594</v>
+      </c>
+      <c r="O18" s="15" t="s">
         <v>1595</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="P18" s="15" t="s">
         <v>1596</v>
-      </c>
-      <c r="P18" s="15" t="s">
-        <v>1597</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -31165,16 +31183,16 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="N20" s="15" t="s">
+        <v>1597</v>
+      </c>
+      <c r="O20" s="15" t="s">
         <v>1598</v>
       </c>
-      <c r="O20" s="15" t="s">
+      <c r="P20" s="15" t="s">
         <v>1599</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>1600</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="64" x14ac:dyDescent="0.2">
@@ -31206,13 +31224,13 @@
         <v>0</v>
       </c>
       <c r="N21" s="15" t="s">
+        <v>1600</v>
+      </c>
+      <c r="O21" s="15" t="s">
         <v>1601</v>
       </c>
-      <c r="O21" s="15" t="s">
+      <c r="P21" s="15" t="s">
         <v>1602</v>
-      </c>
-      <c r="P21" s="15" t="s">
-        <v>1603</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="80" x14ac:dyDescent="0.2">
@@ -31247,10 +31265,10 @@
         <v>1535</v>
       </c>
       <c r="O22" s="15" t="s">
+        <v>1603</v>
+      </c>
+      <c r="P22" s="15" t="s">
         <v>1604</v>
-      </c>
-      <c r="P22" s="15" t="s">
-        <v>1605</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="48" x14ac:dyDescent="0.2">
@@ -31285,10 +31303,10 @@
         <v>1489</v>
       </c>
       <c r="O23" s="15" t="s">
+        <v>1607</v>
+      </c>
+      <c r="P23" s="15" t="s">
         <v>1608</v>
-      </c>
-      <c r="P23" s="15" t="s">
-        <v>1609</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="48" x14ac:dyDescent="0.2">
@@ -31320,13 +31338,13 @@
         <v>0</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="O24" s="15" t="s">
+        <v>1609</v>
+      </c>
+      <c r="P24" s="15" t="s">
         <v>1610</v>
-      </c>
-      <c r="P24" s="15" t="s">
-        <v>1611</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="64" x14ac:dyDescent="0.2">
@@ -31358,13 +31376,13 @@
         <v>0</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="O25" s="15" t="s">
+        <v>1611</v>
+      </c>
+      <c r="P25" s="15" t="s">
         <v>1612</v>
-      </c>
-      <c r="P25" s="15" t="s">
-        <v>1613</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
@@ -44497,7 +44515,7 @@
   <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44891,8 +44909,11 @@
       <c r="I13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -44920,17 +44941,17 @@
       <c r="I14" s="2">
         <v>0</v>
       </c>
-      <c r="O14" s="25" t="s">
+      <c r="O14" s="26" t="s">
         <v>1564</v>
       </c>
-      <c r="P14" s="25" t="s">
+      <c r="P14" s="26" t="s">
+        <v>1631</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>1632</v>
+      </c>
+      <c r="R14" s="26" t="s">
         <v>1583</v>
-      </c>
-      <c r="Q14" s="25" t="s">
-        <v>1615</v>
-      </c>
-      <c r="R14" s="25" t="s">
-        <v>1584</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="64" x14ac:dyDescent="0.2">
@@ -44961,17 +44982,17 @@
       <c r="I15" s="2">
         <v>0</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="25" t="s">
+        <v>1614</v>
+      </c>
+      <c r="P15" s="25" t="s">
+        <v>1595</v>
+      </c>
+      <c r="Q15" s="25" t="s">
+        <v>1615</v>
+      </c>
+      <c r="R15" s="25" t="s">
         <v>1616</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>1596</v>
-      </c>
-      <c r="Q15" s="15" t="s">
-        <v>1617</v>
-      </c>
-      <c r="R15" s="15" t="s">
-        <v>1618</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="64" x14ac:dyDescent="0.2">
@@ -45002,17 +45023,17 @@
       <c r="I16" s="2">
         <v>0</v>
       </c>
-      <c r="O16" s="15" t="s">
-        <v>1619</v>
-      </c>
-      <c r="P16" s="15" t="s">
+      <c r="O16" s="25" t="s">
+        <v>1617</v>
+      </c>
+      <c r="P16" s="25" t="s">
+        <v>1598</v>
+      </c>
+      <c r="Q16" s="25" t="s">
+        <v>1618</v>
+      </c>
+      <c r="R16" s="25" t="s">
         <v>1599</v>
-      </c>
-      <c r="Q16" s="15" t="s">
-        <v>1620</v>
-      </c>
-      <c r="R16" s="15" t="s">
-        <v>1600</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="48" x14ac:dyDescent="0.2">
@@ -45043,20 +45064,20 @@
       <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="O17" s="15" t="s">
+      <c r="O17" s="25" t="s">
+        <v>1600</v>
+      </c>
+      <c r="P17" s="25" t="s">
         <v>1601</v>
       </c>
-      <c r="P17" s="15" t="s">
-        <v>1602</v>
-      </c>
-      <c r="Q17" s="15" t="s">
-        <v>1621</v>
-      </c>
-      <c r="R17" s="15" t="s">
-        <v>1622</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="128" x14ac:dyDescent="0.2">
+      <c r="Q17" s="25" t="s">
+        <v>1619</v>
+      </c>
+      <c r="R17" s="25" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -45084,17 +45105,17 @@
       <c r="I18" s="2">
         <v>0</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="25" t="s">
         <v>1535</v>
       </c>
-      <c r="P18" s="15" t="s">
-        <v>1623</v>
-      </c>
-      <c r="Q18" s="15" t="s">
-        <v>1624</v>
-      </c>
-      <c r="R18" s="15" t="s">
-        <v>1605</v>
+      <c r="P18" s="25" t="s">
+        <v>1621</v>
+      </c>
+      <c r="Q18" s="25" t="s">
+        <v>1622</v>
+      </c>
+      <c r="R18" s="25" t="s">
+        <v>1604</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="48" x14ac:dyDescent="0.2">
@@ -45125,17 +45146,17 @@
       <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="25" t="s">
         <v>1489</v>
       </c>
-      <c r="P19" s="15" t="s">
-        <v>1625</v>
-      </c>
-      <c r="Q19" s="15" t="s">
-        <v>1626</v>
-      </c>
-      <c r="R19" s="15" t="s">
-        <v>1609</v>
+      <c r="P19" s="25" t="s">
+        <v>1623</v>
+      </c>
+      <c r="Q19" s="25" t="s">
+        <v>1624</v>
+      </c>
+      <c r="R19" s="25" t="s">
+        <v>1608</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="64" x14ac:dyDescent="0.2">
@@ -45166,17 +45187,17 @@
       <c r="I20" s="2">
         <v>0</v>
       </c>
-      <c r="O20" s="15" t="s">
-        <v>1606</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>1610</v>
-      </c>
-      <c r="Q20" s="15" t="s">
-        <v>1627</v>
-      </c>
-      <c r="R20" s="15" t="s">
-        <v>1628</v>
+      <c r="O20" s="25" t="s">
+        <v>1605</v>
+      </c>
+      <c r="P20" s="25" t="s">
+        <v>1609</v>
+      </c>
+      <c r="Q20" s="25" t="s">
+        <v>1625</v>
+      </c>
+      <c r="R20" s="25" t="s">
+        <v>1626</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="64" x14ac:dyDescent="0.2">
@@ -45207,17 +45228,17 @@
       <c r="I21" s="2">
         <v>0</v>
       </c>
-      <c r="O21" s="15" t="s">
-        <v>1607</v>
-      </c>
-      <c r="P21" s="15" t="s">
-        <v>1612</v>
-      </c>
-      <c r="Q21" s="15" t="s">
-        <v>1629</v>
-      </c>
-      <c r="R21" s="15" t="s">
-        <v>1630</v>
+      <c r="O21" s="25" t="s">
+        <v>1606</v>
+      </c>
+      <c r="P21" s="25" t="s">
+        <v>1611</v>
+      </c>
+      <c r="Q21" s="25" t="s">
+        <v>1627</v>
+      </c>
+      <c r="R21" s="25" t="s">
+        <v>1628</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -45248,10 +45269,10 @@
       <c r="I22" s="2">
         <v>0</v>
       </c>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">

</xml_diff>